<commit_message>
added Day 8 supporting materials
</commit_message>
<xml_diff>
--- a/Setup and Installation/Angular 14 Lab Setup.xlsx
+++ b/Setup and Installation/Angular 14 Lab Setup.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Serial No.</t>
   </si>
@@ -41,6 +41,123 @@
   </si>
   <si>
     <t>https://code.visualstudio.com/download</t>
+  </si>
+  <si>
+    <t>GitHub Sign Up</t>
+  </si>
+  <si>
+    <t>https://github.com/join</t>
+  </si>
+  <si>
+    <t>Postman</t>
+  </si>
+  <si>
+    <t>https://www.postman.com/downloads/</t>
+  </si>
+  <si>
+    <t>JDK 11 or later</t>
+  </si>
+  <si>
+    <t>https://www.oracle.com/in/java/technologies/javase/jdk11-archive-downloads.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Java 11 and Spring Tool Suite - Setup and Installation.pptx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 'Setup and Installation' folder. </t>
+    </r>
+  </si>
+  <si>
+    <t>Spring Tool Suite 4</t>
+  </si>
+  <si>
+    <t>https://spring.io/tools/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Java 11 and Spring Tool Suite - Setup and Installation.pptx</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 'Setup and Installation' folder. An Eclipse IDE for Java EE can also be installed , if preferred.</t>
+    </r>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>https://www.jenkins.io/download/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Download the LTS Generic Java package (.war). Refer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Jenkins - Setup and Installation.pptx </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in 'Setup and Installation' folder.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -48,12 +165,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,7 +225,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -122,7 +254,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,7 +262,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -151,16 +306,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -176,62 +324,40 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -244,67 +370,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,55 +514,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -376,55 +538,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,23 +582,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,16 +607,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,6 +627,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -538,15 +664,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -559,132 +685,135 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -695,7 +824,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1017,93 +1162,151 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
     <col min="3" max="3" width="76.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="23.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" ht="18.75" spans="1:3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" ht="21" customHeight="1" spans="1:3">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" ht="18.75" spans="1:3">
-      <c r="A7" s="2">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
     </row>
-    <row r="9" ht="18.75" spans="1:2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="7"/>
+    <row r="9" ht="18.75" spans="1:3">
+      <c r="A9" s="3">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
     </row>
-    <row r="11" ht="18.75" spans="1:2">
-      <c r="A11" s="2"/>
-      <c r="B11" s="7"/>
+    <row r="11" ht="18.75" spans="1:3">
+      <c r="A11" s="3">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
     </row>
-    <row r="13" ht="18.75" spans="1:2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="7"/>
+    <row r="13" s="1" customFormat="1" ht="117" customHeight="1" spans="1:4">
+      <c r="A13" s="9">
+        <v>6</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" ht="105" spans="1:4">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" ht="105" spans="1:4">
+      <c r="A17" s="9">
+        <v>8</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" display="https://code.visualstudio.com/download"/>
     <hyperlink ref="C3" r:id="rId2" display="https://git-scm.com/download/win"/>
+    <hyperlink ref="C9" r:id="rId3" display="https://github.com/join"/>
+    <hyperlink ref="C11" r:id="rId4" display="https://www.postman.com/downloads/"/>
+    <hyperlink ref="C13" r:id="rId5" display="https://www.oracle.com/in/java/technologies/javase/jdk11-archive-downloads.html"/>
+    <hyperlink ref="C15" r:id="rId6" display="https://spring.io/tools/"/>
+    <hyperlink ref="C17" r:id="rId7" display="https://www.jenkins.io/download/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
added training materials for final week
</commit_message>
<xml_diff>
--- a/Setup and Installation/Angular 14 Lab Setup.xlsx
+++ b/Setup and Installation/Angular 14 Lab Setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815"/>
+    <workbookView windowWidth="19635" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Lab Setup" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Serial No.</t>
   </si>
@@ -62,6 +62,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Refer </t>
     </r>
     <r>
@@ -95,6 +102,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Refer </t>
     </r>
     <r>
@@ -159,16 +173,25 @@
       <t>in 'Setup and Installation' folder.</t>
     </r>
   </si>
+  <si>
+    <t>Apache Tomcat  version 9</t>
+  </si>
+  <si>
+    <t>https://tomcat.apache.org/download-90.cgi</t>
+  </si>
+  <si>
+    <t>Download the 64-bit Windows zip</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -225,46 +248,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,12 +288,58 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -292,41 +348,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -337,16 +361,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,187 +393,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,6 +584,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -579,11 +635,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -606,47 +668,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -664,152 +687,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -821,8 +844,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -831,67 +854,71 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1162,19 +1189,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="49" customWidth="1"/>
-    <col min="3" max="3" width="76.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="75.5714285714286" customWidth="1"/>
     <col min="4" max="4" width="23.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1296,6 +1323,20 @@
       </c>
       <c r="D17" s="14" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="19" ht="30" spans="1:4">
+      <c r="A19" s="9">
+        <v>5</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1305,8 +1346,9 @@
     <hyperlink ref="C9" r:id="rId3" display="https://github.com/join"/>
     <hyperlink ref="C11" r:id="rId4" display="https://www.postman.com/downloads/"/>
     <hyperlink ref="C13" r:id="rId5" display="https://www.oracle.com/in/java/technologies/javase/jdk11-archive-downloads.html"/>
-    <hyperlink ref="C15" r:id="rId6" display="https://spring.io/tools/"/>
-    <hyperlink ref="C17" r:id="rId7" display="https://www.jenkins.io/download/"/>
+    <hyperlink ref="C17" r:id="rId6" display="https://www.jenkins.io/download/"/>
+    <hyperlink ref="C15" r:id="rId7" display="https://spring.io/tools/"/>
+    <hyperlink ref="C19" r:id="rId8" display="https://tomcat.apache.org/download-90.cgi"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>